<commit_message>
dates were in 2016 but should have been 2023
</commit_message>
<xml_diff>
--- a/data/spuibeheer/extern/verwerkt_in_excel/os_AKL&LK_2023.xlsx
+++ b/data/spuibeheer/extern/verwerkt_in_excel/os_AKL&LK_2023.xlsx
@@ -402,7 +402,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -422,13 +422,9 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="20" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -448,7 +444,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
@@ -767,8 +762,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="I77" sqref="I77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -867,7 +862,7 @@
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A7" s="12">
-        <v>42430</v>
+        <v>44986</v>
       </c>
       <c r="B7" s="12"/>
       <c r="C7" s="13" t="s">
@@ -881,7 +876,7 @@
       <c r="G7" s="16"/>
       <c r="H7" s="16"/>
       <c r="I7" s="17">
-        <v>42430</v>
+        <v>44986</v>
       </c>
       <c r="J7" s="11"/>
       <c r="K7" s="13" t="s">
@@ -897,7 +892,7 @@
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A8" s="12">
-        <v>42431</v>
+        <v>44987</v>
       </c>
       <c r="B8" s="12"/>
       <c r="C8" s="13" t="s">
@@ -910,8 +905,8 @@
       </c>
       <c r="G8" s="16"/>
       <c r="H8" s="16"/>
-      <c r="I8" s="19">
-        <v>42431</v>
+      <c r="I8" s="17">
+        <v>44987</v>
       </c>
       <c r="J8" s="3"/>
       <c r="K8" s="16" t="s">
@@ -923,11 +918,11 @@
         <v>11</v>
       </c>
       <c r="O8" s="16"/>
-      <c r="P8" s="20"/>
+      <c r="P8" s="19"/>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A9" s="12">
-        <v>42432</v>
+        <v>44988</v>
       </c>
       <c r="B9" s="12"/>
       <c r="C9" s="13" t="s">
@@ -940,8 +935,8 @@
       </c>
       <c r="G9" s="16"/>
       <c r="H9" s="16"/>
-      <c r="I9" s="19">
-        <v>42432</v>
+      <c r="I9" s="17">
+        <v>44988</v>
       </c>
       <c r="J9" s="3"/>
       <c r="K9" s="18" t="s">
@@ -953,23 +948,23 @@
         <v>12</v>
       </c>
       <c r="O9" s="16"/>
-      <c r="P9" s="20"/>
+      <c r="P9" s="19"/>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A10" s="12">
-        <v>42433</v>
+        <v>44989</v>
       </c>
       <c r="B10" s="12"/>
       <c r="C10" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="D10" s="31"/>
-      <c r="E10" s="20"/>
+      <c r="D10" s="29"/>
+      <c r="E10" s="19"/>
       <c r="F10" s="16"/>
       <c r="G10" s="16"/>
       <c r="H10" s="16"/>
-      <c r="I10" s="19">
-        <v>42433</v>
+      <c r="I10" s="17">
+        <v>44989</v>
       </c>
       <c r="J10" s="3"/>
       <c r="K10" s="16" t="s">
@@ -979,38 +974,38 @@
       <c r="M10" s="16"/>
       <c r="N10" s="18"/>
       <c r="O10" s="16"/>
-      <c r="P10" s="20"/>
+      <c r="P10" s="19"/>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A11" s="12">
-        <v>42434</v>
+        <v>44990</v>
       </c>
       <c r="B11" s="12"/>
-      <c r="C11" s="32" t="s">
+      <c r="C11" s="30" t="s">
         <v>14</v>
       </c>
       <c r="D11" s="16"/>
-      <c r="E11" s="20"/>
+      <c r="E11" s="19"/>
       <c r="F11" s="16"/>
       <c r="G11" s="16"/>
       <c r="H11" s="16"/>
-      <c r="I11" s="19">
-        <v>42434</v>
-      </c>
-      <c r="K11" s="32" t="s">
+      <c r="I11" s="17">
+        <v>44990</v>
+      </c>
+      <c r="K11" s="30" t="s">
         <v>14</v>
       </c>
       <c r="L11" s="16"/>
       <c r="M11" s="16"/>
       <c r="N11" s="18"/>
       <c r="O11" s="16"/>
-      <c r="P11" s="20"/>
+      <c r="P11" s="19"/>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A12" s="12">
-        <v>42435</v>
-      </c>
-      <c r="B12" s="22"/>
+        <v>44991</v>
+      </c>
+      <c r="B12" s="21"/>
       <c r="C12" s="13" t="s">
         <v>8</v>
       </c>
@@ -1021,8 +1016,8 @@
       </c>
       <c r="G12" s="16"/>
       <c r="H12" s="16"/>
-      <c r="I12" s="19">
-        <v>42435</v>
+      <c r="I12" s="17">
+        <v>44991</v>
       </c>
       <c r="K12" s="18" t="s">
         <v>13</v>
@@ -1031,25 +1026,25 @@
       <c r="M12" s="16"/>
       <c r="N12" s="18"/>
       <c r="O12" s="16"/>
-      <c r="P12" s="20"/>
+      <c r="P12" s="19"/>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A13" s="12">
-        <v>42436</v>
+        <v>44992</v>
       </c>
       <c r="B13" s="12"/>
       <c r="C13" s="18" t="s">
         <v>8</v>
       </c>
       <c r="D13" s="16"/>
-      <c r="E13" s="20"/>
+      <c r="E13" s="19"/>
       <c r="F13" s="18" t="s">
         <v>8</v>
       </c>
       <c r="G13" s="16"/>
       <c r="H13" s="16"/>
-      <c r="I13" s="19">
-        <v>42436</v>
+      <c r="I13" s="17">
+        <v>44992</v>
       </c>
       <c r="K13" s="18" t="s">
         <v>36</v>
@@ -1060,25 +1055,25 @@
         <v>15</v>
       </c>
       <c r="O13" s="16"/>
-      <c r="P13" s="20"/>
+      <c r="P13" s="19"/>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A14" s="12">
-        <v>42437</v>
+        <v>44993</v>
       </c>
       <c r="B14" s="12"/>
       <c r="C14" s="18" t="s">
         <v>8</v>
       </c>
       <c r="D14" s="16"/>
-      <c r="E14" s="20"/>
+      <c r="E14" s="19"/>
       <c r="F14" s="18" t="s">
         <v>8</v>
       </c>
       <c r="G14" s="16"/>
       <c r="H14" s="16"/>
-      <c r="I14" s="19">
-        <v>42437</v>
+      <c r="I14" s="17">
+        <v>44993</v>
       </c>
       <c r="K14" s="18" t="s">
         <v>13</v>
@@ -1087,11 +1082,11 @@
       <c r="M14" s="16"/>
       <c r="N14" s="18"/>
       <c r="O14" s="16"/>
-      <c r="P14" s="20"/>
+      <c r="P14" s="19"/>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A15" s="12">
-        <v>42438</v>
+        <v>44994</v>
       </c>
       <c r="B15" s="12"/>
       <c r="C15" s="13" t="s">
@@ -1104,8 +1099,8 @@
       </c>
       <c r="G15" s="16"/>
       <c r="H15" s="16"/>
-      <c r="I15" s="19">
-        <v>42438</v>
+      <c r="I15" s="17">
+        <v>44994</v>
       </c>
       <c r="K15" s="18" t="s">
         <v>13</v>
@@ -1114,25 +1109,25 @@
       <c r="M15" s="16"/>
       <c r="N15" s="18"/>
       <c r="O15" s="16"/>
-      <c r="P15" s="20"/>
+      <c r="P15" s="19"/>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A16" s="12">
-        <v>42439</v>
+        <v>44995</v>
       </c>
       <c r="B16" s="12"/>
-      <c r="C16" s="21" t="s">
+      <c r="C16" s="20" t="s">
         <v>8</v>
       </c>
       <c r="D16" s="16"/>
-      <c r="E16" s="20"/>
+      <c r="E16" s="19"/>
       <c r="F16" s="18" t="s">
         <v>8</v>
       </c>
       <c r="G16" s="16"/>
       <c r="H16" s="16"/>
-      <c r="I16" s="19">
-        <v>42439</v>
+      <c r="I16" s="17">
+        <v>44995</v>
       </c>
       <c r="K16" s="18" t="s">
         <v>13</v>
@@ -1141,11 +1136,11 @@
       <c r="M16" s="16"/>
       <c r="N16" s="18"/>
       <c r="O16" s="16"/>
-      <c r="P16" s="20"/>
+      <c r="P16" s="19"/>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A17" s="12">
-        <v>42440</v>
+        <v>44996</v>
       </c>
       <c r="B17" s="12"/>
       <c r="C17" s="18" t="s">
@@ -1156,8 +1151,8 @@
       <c r="F17" s="18"/>
       <c r="G17" s="16"/>
       <c r="H17" s="16"/>
-      <c r="I17" s="19">
-        <v>42440</v>
+      <c r="I17" s="17">
+        <v>44996</v>
       </c>
       <c r="K17" s="18" t="s">
         <v>16</v>
@@ -1166,14 +1161,14 @@
       <c r="M17" s="16"/>
       <c r="N17" s="18"/>
       <c r="O17" s="16"/>
-      <c r="P17" s="20"/>
+      <c r="P17" s="19"/>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A18" s="12">
-        <v>42441</v>
+        <v>44997</v>
       </c>
       <c r="B18" s="12"/>
-      <c r="C18" s="32" t="s">
+      <c r="C18" s="30" t="s">
         <v>14</v>
       </c>
       <c r="D18" s="16"/>
@@ -1181,35 +1176,35 @@
       <c r="F18" s="18"/>
       <c r="G18" s="16"/>
       <c r="H18" s="16"/>
-      <c r="I18" s="19">
-        <v>42441</v>
-      </c>
-      <c r="K18" s="32" t="s">
+      <c r="I18" s="17">
+        <v>44997</v>
+      </c>
+      <c r="K18" s="30" t="s">
         <v>14</v>
       </c>
       <c r="L18" s="16"/>
       <c r="M18" s="16"/>
       <c r="N18" s="18"/>
       <c r="O18" s="16"/>
-      <c r="P18" s="20"/>
+      <c r="P18" s="19"/>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A19" s="12">
-        <v>42442</v>
+        <v>44998</v>
       </c>
       <c r="B19" s="12"/>
-      <c r="C19" s="21" t="s">
+      <c r="C19" s="20" t="s">
         <v>8</v>
       </c>
       <c r="D19" s="16"/>
-      <c r="E19" s="20"/>
+      <c r="E19" s="19"/>
       <c r="F19" s="18" t="s">
         <v>8</v>
       </c>
       <c r="G19" s="16"/>
       <c r="H19" s="16"/>
-      <c r="I19" s="19">
-        <v>42442</v>
+      <c r="I19" s="17">
+        <v>44998</v>
       </c>
       <c r="K19" s="18" t="s">
         <v>9</v>
@@ -1220,11 +1215,11 @@
         <v>17</v>
       </c>
       <c r="O19" s="16"/>
-      <c r="P19" s="20"/>
+      <c r="P19" s="19"/>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A20" s="12">
-        <v>42443</v>
+        <v>44999</v>
       </c>
       <c r="B20" s="12"/>
       <c r="C20" s="18" t="s">
@@ -1237,8 +1232,8 @@
       </c>
       <c r="G20" s="16"/>
       <c r="H20" s="16"/>
-      <c r="I20" s="19">
-        <v>42443</v>
+      <c r="I20" s="17">
+        <v>44999</v>
       </c>
       <c r="K20" s="18" t="s">
         <v>16</v>
@@ -1247,11 +1242,11 @@
       <c r="M20" s="16"/>
       <c r="N20" s="18"/>
       <c r="O20" s="16"/>
-      <c r="P20" s="20"/>
+      <c r="P20" s="19"/>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A21" s="12">
-        <v>42444</v>
+        <v>45000</v>
       </c>
       <c r="B21" s="12"/>
       <c r="C21" s="18" t="s">
@@ -1264,22 +1259,22 @@
       </c>
       <c r="G21" s="16"/>
       <c r="H21" s="16"/>
-      <c r="I21" s="23">
-        <v>42444</v>
-      </c>
-      <c r="J21" s="24"/>
+      <c r="I21" s="17">
+        <v>45000</v>
+      </c>
+      <c r="J21" s="22"/>
       <c r="K21" s="18" t="s">
         <v>13</v>
       </c>
       <c r="L21" s="16"/>
-      <c r="M21" s="26"/>
-      <c r="N21" s="25"/>
+      <c r="M21" s="24"/>
+      <c r="N21" s="23"/>
       <c r="O21" s="16"/>
-      <c r="P21" s="20"/>
+      <c r="P21" s="19"/>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A22" s="12">
-        <v>42445</v>
+        <v>45001</v>
       </c>
       <c r="B22" s="12"/>
       <c r="C22" s="18" t="s">
@@ -1292,8 +1287,8 @@
       </c>
       <c r="G22" s="16"/>
       <c r="H22" s="16"/>
-      <c r="I22" s="19">
-        <v>42445</v>
+      <c r="I22" s="17">
+        <v>45001</v>
       </c>
       <c r="K22" s="18" t="s">
         <v>13</v>
@@ -1302,11 +1297,11 @@
       <c r="M22" s="16"/>
       <c r="N22" s="18"/>
       <c r="O22" s="16"/>
-      <c r="P22" s="20"/>
+      <c r="P22" s="19"/>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A23" s="12">
-        <v>42446</v>
+        <v>45002</v>
       </c>
       <c r="B23" s="12"/>
       <c r="C23" s="18" t="s">
@@ -1317,10 +1312,10 @@
       <c r="F23" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="G23" s="27"/>
-      <c r="H23" s="27"/>
-      <c r="I23" s="19">
-        <v>42446</v>
+      <c r="G23" s="25"/>
+      <c r="H23" s="25"/>
+      <c r="I23" s="17">
+        <v>45002</v>
       </c>
       <c r="K23" s="18" t="s">
         <v>16</v>
@@ -1329,14 +1324,14 @@
       <c r="M23" s="16"/>
       <c r="N23" s="18"/>
       <c r="O23" s="16"/>
-      <c r="P23" s="20"/>
+      <c r="P23" s="19"/>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A24" s="12">
-        <v>42447</v>
+        <v>45003</v>
       </c>
       <c r="B24" s="12"/>
-      <c r="C24" s="21" t="s">
+      <c r="C24" s="20" t="s">
         <v>20</v>
       </c>
       <c r="D24" s="16"/>
@@ -1344,10 +1339,10 @@
       <c r="F24" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="G24" s="27"/>
-      <c r="H24" s="27"/>
-      <c r="I24" s="19">
-        <v>42447</v>
+      <c r="G24" s="25"/>
+      <c r="H24" s="25"/>
+      <c r="I24" s="17">
+        <v>45003</v>
       </c>
       <c r="K24" s="18" t="s">
         <v>20</v>
@@ -1358,14 +1353,14 @@
         <v>11</v>
       </c>
       <c r="O24" s="16"/>
-      <c r="P24" s="20"/>
+      <c r="P24" s="19"/>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A25" s="12">
-        <v>42448</v>
+        <v>45004</v>
       </c>
       <c r="B25" s="12"/>
-      <c r="C25" s="32" t="s">
+      <c r="C25" s="30" t="s">
         <v>14</v>
       </c>
       <c r="D25" s="16"/>
@@ -1373,22 +1368,22 @@
       <c r="F25" s="18"/>
       <c r="G25" s="16"/>
       <c r="H25" s="16"/>
-      <c r="I25" s="19">
-        <v>42448</v>
+      <c r="I25" s="17">
+        <v>45004</v>
       </c>
       <c r="J25" s="16"/>
-      <c r="K25" s="32" t="s">
+      <c r="K25" s="30" t="s">
         <v>14</v>
       </c>
       <c r="L25" s="16"/>
       <c r="M25" s="16"/>
       <c r="N25" s="18"/>
       <c r="O25" s="16"/>
-      <c r="P25" s="20"/>
+      <c r="P25" s="19"/>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A26" s="12">
-        <v>42449</v>
+        <v>45005</v>
       </c>
       <c r="B26" s="12"/>
       <c r="C26" s="18" t="s">
@@ -1401,8 +1396,8 @@
       </c>
       <c r="G26" s="16"/>
       <c r="H26" s="16"/>
-      <c r="I26" s="19">
-        <v>42449</v>
+      <c r="I26" s="17">
+        <v>45005</v>
       </c>
       <c r="J26" s="16"/>
       <c r="K26" s="18" t="s">
@@ -1412,11 +1407,11 @@
       <c r="M26" s="16"/>
       <c r="N26" s="18"/>
       <c r="O26" s="16"/>
-      <c r="P26" s="20"/>
+      <c r="P26" s="19"/>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A27" s="12">
-        <v>42450</v>
+        <v>45006</v>
       </c>
       <c r="B27" s="12"/>
       <c r="C27" s="18" t="s">
@@ -1429,8 +1424,8 @@
       </c>
       <c r="G27" s="16"/>
       <c r="H27" s="16"/>
-      <c r="I27" s="19">
-        <v>42450</v>
+      <c r="I27" s="17">
+        <v>45006</v>
       </c>
       <c r="J27" s="16"/>
       <c r="K27" s="18" t="s">
@@ -1440,11 +1435,11 @@
       <c r="M27" s="16"/>
       <c r="N27" s="18"/>
       <c r="O27" s="16"/>
-      <c r="P27" s="20"/>
+      <c r="P27" s="19"/>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A28" s="12">
-        <v>42451</v>
+        <v>45007</v>
       </c>
       <c r="B28" s="12"/>
       <c r="C28" s="18" t="s">
@@ -1457,8 +1452,8 @@
       </c>
       <c r="G28" s="16"/>
       <c r="H28" s="16"/>
-      <c r="I28" s="19">
-        <v>42451</v>
+      <c r="I28" s="17">
+        <v>45007</v>
       </c>
       <c r="J28" s="16"/>
       <c r="K28" s="18" t="s">
@@ -1468,11 +1463,11 @@
       <c r="M28" s="16"/>
       <c r="N28" s="18"/>
       <c r="O28" s="16"/>
-      <c r="P28" s="20"/>
+      <c r="P28" s="19"/>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A29" s="12">
-        <v>42452</v>
+        <v>45008</v>
       </c>
       <c r="B29" s="12"/>
       <c r="C29" s="18" t="s">
@@ -1485,8 +1480,8 @@
       </c>
       <c r="G29" s="16"/>
       <c r="H29" s="16"/>
-      <c r="I29" s="19">
-        <v>42452</v>
+      <c r="I29" s="17">
+        <v>45008</v>
       </c>
       <c r="J29" s="16"/>
       <c r="K29" s="18" t="s">
@@ -1496,11 +1491,11 @@
       <c r="M29" s="16"/>
       <c r="N29" s="18"/>
       <c r="O29" s="16"/>
-      <c r="P29" s="20"/>
+      <c r="P29" s="19"/>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A30" s="12">
-        <v>42453</v>
+        <v>45009</v>
       </c>
       <c r="B30" s="12"/>
       <c r="C30" s="18"/>
@@ -1509,8 +1504,8 @@
       <c r="F30" s="18"/>
       <c r="G30" s="16"/>
       <c r="H30" s="16"/>
-      <c r="I30" s="19">
-        <v>42453</v>
+      <c r="I30" s="17">
+        <v>45009</v>
       </c>
       <c r="J30" s="16"/>
       <c r="K30" s="18"/>
@@ -1518,23 +1513,23 @@
       <c r="M30" s="16"/>
       <c r="N30" s="18"/>
       <c r="O30" s="16"/>
-      <c r="P30" s="20"/>
+      <c r="P30" s="19"/>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A31" s="12">
-        <v>42454</v>
+        <v>45010</v>
       </c>
       <c r="B31" s="12"/>
-      <c r="C31" s="34" t="s">
+      <c r="C31" s="32" t="s">
         <v>22</v>
       </c>
       <c r="D31" s="16"/>
       <c r="E31" s="16"/>
-      <c r="F31" s="21"/>
+      <c r="F31" s="20"/>
       <c r="G31" s="16"/>
       <c r="H31" s="16"/>
-      <c r="I31" s="19">
-        <v>42454</v>
+      <c r="I31" s="17">
+        <v>45010</v>
       </c>
       <c r="J31" s="16"/>
       <c r="K31" s="18" t="s">
@@ -1542,41 +1537,41 @@
       </c>
       <c r="L31" s="16"/>
       <c r="M31" s="16"/>
-      <c r="N31" s="21" t="s">
+      <c r="N31" s="20" t="s">
         <v>57</v>
       </c>
       <c r="O31" s="16"/>
-      <c r="P31" s="20"/>
+      <c r="P31" s="19"/>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A32" s="12">
-        <v>42455</v>
+        <v>45011</v>
       </c>
       <c r="B32" s="12"/>
-      <c r="C32" s="32" t="s">
+      <c r="C32" s="30" t="s">
         <v>14</v>
       </c>
       <c r="D32" s="16"/>
       <c r="E32" s="16"/>
-      <c r="F32" s="21"/>
+      <c r="F32" s="20"/>
       <c r="G32" s="16"/>
       <c r="H32" s="16"/>
-      <c r="I32" s="19">
-        <v>42455</v>
+      <c r="I32" s="17">
+        <v>45011</v>
       </c>
       <c r="J32" s="16"/>
-      <c r="K32" s="32" t="s">
+      <c r="K32" s="30" t="s">
         <v>24</v>
       </c>
       <c r="L32" s="16"/>
       <c r="M32" s="16"/>
       <c r="N32" s="18"/>
       <c r="O32" s="16"/>
-      <c r="P32" s="20"/>
+      <c r="P32" s="19"/>
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A33" s="12">
-        <v>42456</v>
+        <v>45012</v>
       </c>
       <c r="B33" s="12"/>
       <c r="C33" s="18" t="s">
@@ -1589,8 +1584,8 @@
       </c>
       <c r="G33" s="16"/>
       <c r="H33" s="16"/>
-      <c r="I33" s="19">
-        <v>42456</v>
+      <c r="I33" s="17">
+        <v>45012</v>
       </c>
       <c r="J33" s="16"/>
       <c r="K33" s="18" t="s">
@@ -1602,14 +1597,14 @@
         <v>23</v>
       </c>
       <c r="O33" s="16"/>
-      <c r="P33" s="20"/>
+      <c r="P33" s="19"/>
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A34" s="12">
-        <v>42457</v>
+        <v>45013</v>
       </c>
       <c r="B34" s="12"/>
-      <c r="C34" s="21" t="s">
+      <c r="C34" s="20" t="s">
         <v>18</v>
       </c>
       <c r="D34" s="16"/>
@@ -1619,8 +1614,8 @@
       </c>
       <c r="G34" s="16"/>
       <c r="H34" s="16"/>
-      <c r="I34" s="19">
-        <v>42457</v>
+      <c r="I34" s="17">
+        <v>45013</v>
       </c>
       <c r="J34" s="16"/>
       <c r="K34" s="18" t="s">
@@ -1628,29 +1623,29 @@
       </c>
       <c r="L34" s="16"/>
       <c r="M34" s="16"/>
-      <c r="N34" s="33" t="s">
+      <c r="N34" s="31" t="s">
         <v>55</v>
       </c>
       <c r="O34" s="16"/>
-      <c r="P34" s="20"/>
+      <c r="P34" s="19"/>
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A35" s="12">
-        <v>42458</v>
+        <v>45014</v>
       </c>
       <c r="B35" s="12"/>
-      <c r="C35" s="21" t="s">
+      <c r="C35" s="20" t="s">
         <v>18</v>
       </c>
       <c r="D35" s="16"/>
       <c r="E35" s="16"/>
-      <c r="F35" s="21" t="s">
+      <c r="F35" s="20" t="s">
         <v>18</v>
       </c>
       <c r="G35" s="16"/>
       <c r="H35" s="16"/>
-      <c r="I35" s="19">
-        <v>42458</v>
+      <c r="I35" s="17">
+        <v>45014</v>
       </c>
       <c r="J35" s="16"/>
       <c r="K35" s="18" t="s">
@@ -1658,29 +1653,29 @@
       </c>
       <c r="L35" s="16"/>
       <c r="M35" s="16"/>
-      <c r="N35" s="21" t="s">
+      <c r="N35" s="20" t="s">
         <v>54</v>
       </c>
       <c r="O35" s="16"/>
-      <c r="P35" s="20"/>
+      <c r="P35" s="19"/>
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A36" s="12">
-        <v>42459</v>
+        <v>45015</v>
       </c>
       <c r="B36" s="12"/>
-      <c r="C36" s="21" t="s">
+      <c r="C36" s="20" t="s">
         <v>18</v>
       </c>
       <c r="D36" s="16"/>
       <c r="E36" s="16"/>
-      <c r="F36" s="21" t="s">
+      <c r="F36" s="20" t="s">
         <v>18</v>
       </c>
       <c r="G36" s="16"/>
       <c r="H36" s="16"/>
-      <c r="I36" s="19">
-        <v>42459</v>
+      <c r="I36" s="17">
+        <v>45015</v>
       </c>
       <c r="J36" s="16"/>
       <c r="K36" s="18" t="s">
@@ -1688,15 +1683,15 @@
       </c>
       <c r="L36" s="16"/>
       <c r="M36" s="16"/>
-      <c r="N36" s="21" t="s">
+      <c r="N36" s="20" t="s">
         <v>53</v>
       </c>
       <c r="O36" s="16"/>
-      <c r="P36" s="20"/>
+      <c r="P36" s="19"/>
     </row>
     <row r="37" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A37" s="12">
-        <v>42460</v>
+        <v>45016</v>
       </c>
       <c r="B37" s="12"/>
       <c r="C37" s="18" t="s">
@@ -1709,8 +1704,8 @@
       </c>
       <c r="G37" s="16"/>
       <c r="H37" s="16"/>
-      <c r="I37" s="19">
-        <v>42460</v>
+      <c r="I37" s="17">
+        <v>45016</v>
       </c>
       <c r="J37" s="16"/>
       <c r="K37" s="18" t="s">
@@ -1722,11 +1717,11 @@
         <v>52</v>
       </c>
       <c r="O37" s="16"/>
-      <c r="P37" s="20"/>
+      <c r="P37" s="19"/>
     </row>
     <row r="38" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A38" s="12">
-        <v>42461</v>
+        <v>45017</v>
       </c>
       <c r="B38" s="12"/>
       <c r="C38" s="18" t="s">
@@ -1737,8 +1732,8 @@
       <c r="F38" s="18"/>
       <c r="G38" s="16"/>
       <c r="H38" s="16"/>
-      <c r="I38" s="19">
-        <v>42461</v>
+      <c r="I38" s="17">
+        <v>45017</v>
       </c>
       <c r="J38" s="16"/>
       <c r="K38" s="18" t="s">
@@ -1748,14 +1743,14 @@
       <c r="M38" s="16"/>
       <c r="N38" s="18"/>
       <c r="O38" s="16"/>
-      <c r="P38" s="20"/>
+      <c r="P38" s="19"/>
     </row>
     <row r="39" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A39" s="12">
-        <v>42462</v>
+        <v>45018</v>
       </c>
       <c r="B39" s="12"/>
-      <c r="C39" s="32" t="s">
+      <c r="C39" s="30" t="s">
         <v>14</v>
       </c>
       <c r="D39" s="16"/>
@@ -1763,22 +1758,22 @@
       <c r="F39" s="18"/>
       <c r="G39" s="16"/>
       <c r="H39" s="16"/>
-      <c r="I39" s="19">
-        <v>42462</v>
+      <c r="I39" s="17">
+        <v>45018</v>
       </c>
       <c r="J39" s="16"/>
-      <c r="K39" s="32" t="s">
+      <c r="K39" s="30" t="s">
         <v>14</v>
       </c>
       <c r="L39" s="16"/>
       <c r="M39" s="16"/>
       <c r="N39" s="18"/>
       <c r="O39" s="16"/>
-      <c r="P39" s="20"/>
+      <c r="P39" s="19"/>
     </row>
     <row r="40" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A40" s="12">
-        <v>42463</v>
+        <v>45019</v>
       </c>
       <c r="B40" s="12"/>
       <c r="C40" s="16" t="s">
@@ -1790,8 +1785,8 @@
       </c>
       <c r="G40" s="16"/>
       <c r="H40" s="16"/>
-      <c r="I40" s="19">
-        <v>42463</v>
+      <c r="I40" s="17">
+        <v>45019</v>
       </c>
       <c r="J40" s="16"/>
       <c r="K40" s="16" t="s">
@@ -1801,11 +1796,11 @@
       <c r="M40" s="16"/>
       <c r="N40" s="18"/>
       <c r="O40" s="16"/>
-      <c r="P40" s="20"/>
+      <c r="P40" s="19"/>
     </row>
     <row r="41" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A41" s="12">
-        <v>42464</v>
+        <v>45020</v>
       </c>
       <c r="B41" s="12"/>
       <c r="C41" s="18" t="s">
@@ -1818,8 +1813,8 @@
       </c>
       <c r="G41" s="16"/>
       <c r="H41" s="16"/>
-      <c r="I41" s="19">
-        <v>42464</v>
+      <c r="I41" s="17">
+        <v>45020</v>
       </c>
       <c r="J41" s="16"/>
       <c r="K41" s="18" t="s">
@@ -1831,11 +1826,11 @@
         <v>50</v>
       </c>
       <c r="O41" s="16"/>
-      <c r="P41" s="20"/>
+      <c r="P41" s="19"/>
     </row>
     <row r="42" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A42" s="12">
-        <v>42465</v>
+        <v>45021</v>
       </c>
       <c r="B42" s="12"/>
       <c r="C42" s="18" t="s">
@@ -1848,8 +1843,8 @@
       </c>
       <c r="G42" s="16"/>
       <c r="H42" s="16"/>
-      <c r="I42" s="19">
-        <v>42465</v>
+      <c r="I42" s="17">
+        <v>45021</v>
       </c>
       <c r="J42" s="16"/>
       <c r="K42" s="18" t="s">
@@ -1861,11 +1856,11 @@
         <v>50</v>
       </c>
       <c r="O42" s="16"/>
-      <c r="P42" s="20"/>
+      <c r="P42" s="19"/>
     </row>
     <row r="43" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A43" s="12">
-        <v>42466</v>
+        <v>45022</v>
       </c>
       <c r="B43" s="12"/>
       <c r="C43" s="18" t="s">
@@ -1878,8 +1873,8 @@
       </c>
       <c r="G43" s="16"/>
       <c r="H43" s="16"/>
-      <c r="I43" s="19">
-        <v>42466</v>
+      <c r="I43" s="17">
+        <v>45022</v>
       </c>
       <c r="J43" s="16"/>
       <c r="K43" s="18" t="s">
@@ -1891,11 +1886,11 @@
         <v>43</v>
       </c>
       <c r="O43" s="16"/>
-      <c r="P43" s="20"/>
+      <c r="P43" s="19"/>
     </row>
     <row r="44" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A44" s="12">
-        <v>42467</v>
+        <v>45023</v>
       </c>
       <c r="B44" s="12"/>
       <c r="C44" s="18" t="s">
@@ -1906,8 +1901,8 @@
       <c r="F44" s="18"/>
       <c r="G44" s="16"/>
       <c r="H44" s="16"/>
-      <c r="I44" s="19">
-        <v>42467</v>
+      <c r="I44" s="17">
+        <v>45023</v>
       </c>
       <c r="J44" s="16"/>
       <c r="K44" s="18" t="s">
@@ -1917,11 +1912,11 @@
       <c r="M44" s="16"/>
       <c r="N44" s="18"/>
       <c r="O44" s="16"/>
-      <c r="P44" s="20"/>
+      <c r="P44" s="19"/>
     </row>
     <row r="45" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A45" s="12">
-        <v>42468</v>
+        <v>45024</v>
       </c>
       <c r="B45" s="12"/>
       <c r="C45" s="18" t="s">
@@ -1932,8 +1927,8 @@
       <c r="F45" s="18"/>
       <c r="G45" s="16"/>
       <c r="H45" s="16"/>
-      <c r="I45" s="19">
-        <v>42468</v>
+      <c r="I45" s="17">
+        <v>45024</v>
       </c>
       <c r="J45" s="16"/>
       <c r="K45" s="18" t="s">
@@ -1943,14 +1938,14 @@
       <c r="M45" s="16"/>
       <c r="N45" s="18"/>
       <c r="O45" s="16"/>
-      <c r="P45" s="20"/>
+      <c r="P45" s="19"/>
     </row>
     <row r="46" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A46" s="12">
-        <v>42469</v>
+        <v>45025</v>
       </c>
       <c r="B46" s="12"/>
-      <c r="C46" s="32" t="s">
+      <c r="C46" s="30" t="s">
         <v>14</v>
       </c>
       <c r="D46" s="16"/>
@@ -1958,33 +1953,33 @@
       <c r="F46" s="18"/>
       <c r="G46" s="16"/>
       <c r="H46" s="16"/>
-      <c r="I46" s="19">
-        <v>42469</v>
+      <c r="I46" s="17">
+        <v>45025</v>
       </c>
       <c r="J46" s="16"/>
-      <c r="K46" s="32" t="s">
+      <c r="K46" s="30" t="s">
         <v>24</v>
       </c>
       <c r="L46" s="16"/>
       <c r="M46" s="16"/>
       <c r="N46" s="18"/>
       <c r="O46" s="16"/>
-      <c r="P46" s="20"/>
+      <c r="P46" s="19"/>
     </row>
     <row r="47" spans="1:16" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A47" s="12">
-        <v>42470</v>
+        <v>45026</v>
       </c>
       <c r="B47" s="12"/>
       <c r="C47" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="E47" s="28"/>
+      <c r="E47" s="26"/>
       <c r="F47" s="18"/>
       <c r="G47" s="16"/>
       <c r="H47" s="16"/>
-      <c r="I47" s="19">
-        <v>42470</v>
+      <c r="I47" s="17">
+        <v>45026</v>
       </c>
       <c r="J47" s="16"/>
       <c r="K47" s="18" t="s">
@@ -1994,11 +1989,11 @@
       <c r="M47" s="16"/>
       <c r="N47" s="18"/>
       <c r="O47" s="16"/>
-      <c r="P47" s="20"/>
+      <c r="P47" s="19"/>
     </row>
     <row r="48" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A48" s="12">
-        <v>42471</v>
+        <v>45027</v>
       </c>
       <c r="B48" s="12"/>
       <c r="C48" s="18" t="s">
@@ -2011,8 +2006,8 @@
       </c>
       <c r="G48" s="16"/>
       <c r="H48" s="16"/>
-      <c r="I48" s="19">
-        <v>42471</v>
+      <c r="I48" s="17">
+        <v>45027</v>
       </c>
       <c r="J48" s="16"/>
       <c r="K48" s="18" t="s">
@@ -2022,11 +2017,11 @@
       <c r="M48" s="16"/>
       <c r="N48" s="18"/>
       <c r="O48" s="16"/>
-      <c r="P48" s="20"/>
+      <c r="P48" s="19"/>
     </row>
     <row r="49" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A49" s="12">
-        <v>42472</v>
+        <v>45028</v>
       </c>
       <c r="B49" s="12"/>
       <c r="C49" s="18" t="s">
@@ -2039,8 +2034,8 @@
       </c>
       <c r="G49" s="16"/>
       <c r="H49" s="16"/>
-      <c r="I49" s="19">
-        <v>42472</v>
+      <c r="I49" s="17">
+        <v>45028</v>
       </c>
       <c r="J49" s="16"/>
       <c r="K49" s="18" t="s">
@@ -2050,11 +2045,11 @@
       <c r="M49" s="16"/>
       <c r="N49" s="18"/>
       <c r="O49" s="16"/>
-      <c r="P49" s="20"/>
+      <c r="P49" s="19"/>
     </row>
     <row r="50" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A50" s="12">
-        <v>42473</v>
+        <v>45029</v>
       </c>
       <c r="B50" s="12"/>
       <c r="C50" s="18" t="s">
@@ -2067,22 +2062,22 @@
       </c>
       <c r="G50" s="16"/>
       <c r="H50" s="16"/>
-      <c r="I50" s="19">
-        <v>42473</v>
+      <c r="I50" s="17">
+        <v>45029</v>
       </c>
       <c r="J50" s="16"/>
-      <c r="K50" s="21" t="s">
+      <c r="K50" s="20" t="s">
         <v>27</v>
       </c>
       <c r="L50" s="16"/>
       <c r="M50" s="16"/>
-      <c r="N50" s="21"/>
+      <c r="N50" s="20"/>
       <c r="O50" s="16"/>
-      <c r="P50" s="20"/>
+      <c r="P50" s="19"/>
     </row>
     <row r="51" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A51" s="12">
-        <v>42474</v>
+        <v>45030</v>
       </c>
       <c r="B51" s="12"/>
       <c r="C51" s="18" t="s">
@@ -2095,8 +2090,8 @@
       </c>
       <c r="G51" s="16"/>
       <c r="H51" s="16"/>
-      <c r="I51" s="19">
-        <v>42474</v>
+      <c r="I51" s="17">
+        <v>45030</v>
       </c>
       <c r="J51" s="16"/>
       <c r="K51" s="18" t="s">
@@ -2106,11 +2101,11 @@
       <c r="M51" s="16"/>
       <c r="N51" s="18"/>
       <c r="O51" s="16"/>
-      <c r="P51" s="20"/>
+      <c r="P51" s="19"/>
     </row>
     <row r="52" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A52" s="12">
-        <v>42475</v>
+        <v>45031</v>
       </c>
       <c r="B52" s="12"/>
       <c r="C52" s="18" t="s">
@@ -2121,8 +2116,8 @@
       <c r="F52" s="18"/>
       <c r="G52" s="16"/>
       <c r="H52" s="16"/>
-      <c r="I52" s="19">
-        <v>42475</v>
+      <c r="I52" s="17">
+        <v>45031</v>
       </c>
       <c r="J52" s="16"/>
       <c r="K52" s="18" t="s">
@@ -2132,14 +2127,14 @@
       <c r="M52" s="16"/>
       <c r="N52" s="18"/>
       <c r="O52" s="16"/>
-      <c r="P52" s="20"/>
+      <c r="P52" s="19"/>
     </row>
     <row r="53" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A53" s="12">
-        <v>42476</v>
+        <v>45032</v>
       </c>
       <c r="B53" s="12"/>
-      <c r="C53" s="32" t="s">
+      <c r="C53" s="30" t="s">
         <v>14</v>
       </c>
       <c r="D53" s="16"/>
@@ -2147,22 +2142,22 @@
       <c r="F53" s="18"/>
       <c r="G53" s="16"/>
       <c r="H53" s="16"/>
-      <c r="I53" s="19">
-        <v>42476</v>
+      <c r="I53" s="17">
+        <v>45032</v>
       </c>
       <c r="J53" s="16"/>
-      <c r="K53" s="32" t="s">
+      <c r="K53" s="30" t="s">
         <v>14</v>
       </c>
       <c r="L53" s="16"/>
       <c r="M53" s="16"/>
       <c r="N53" s="18"/>
       <c r="O53" s="16"/>
-      <c r="P53" s="20"/>
+      <c r="P53" s="19"/>
     </row>
     <row r="54" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A54" s="12">
-        <v>42477</v>
+        <v>45033</v>
       </c>
       <c r="B54" s="12"/>
       <c r="C54" s="18" t="s">
@@ -2175,8 +2170,8 @@
       </c>
       <c r="G54" s="16"/>
       <c r="H54" s="16"/>
-      <c r="I54" s="19">
-        <v>42477</v>
+      <c r="I54" s="17">
+        <v>45033</v>
       </c>
       <c r="J54" s="16"/>
       <c r="K54" s="18" t="s">
@@ -2186,11 +2181,11 @@
       <c r="M54" s="16"/>
       <c r="N54" s="18"/>
       <c r="O54" s="16"/>
-      <c r="P54" s="20"/>
+      <c r="P54" s="19"/>
     </row>
     <row r="55" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A55" s="12">
-        <v>42478</v>
+        <v>45034</v>
       </c>
       <c r="B55" s="12"/>
       <c r="C55" s="18" t="s">
@@ -2203,8 +2198,8 @@
       </c>
       <c r="G55" s="16"/>
       <c r="H55" s="16"/>
-      <c r="I55" s="19">
-        <v>42478</v>
+      <c r="I55" s="17">
+        <v>45034</v>
       </c>
       <c r="J55" s="16"/>
       <c r="K55" s="18" t="s">
@@ -2214,11 +2209,11 @@
       <c r="M55" s="16"/>
       <c r="N55" s="18"/>
       <c r="O55" s="16"/>
-      <c r="P55" s="20"/>
+      <c r="P55" s="19"/>
     </row>
     <row r="56" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A56" s="12">
-        <v>42479</v>
+        <v>45035</v>
       </c>
       <c r="B56" s="12"/>
       <c r="C56" s="18" t="s">
@@ -2231,8 +2226,8 @@
       </c>
       <c r="G56" s="16"/>
       <c r="H56" s="16"/>
-      <c r="I56" s="19">
-        <v>42479</v>
+      <c r="I56" s="17">
+        <v>45035</v>
       </c>
       <c r="J56" s="16"/>
       <c r="K56" s="18" t="s">
@@ -2242,11 +2237,11 @@
       <c r="M56" s="16"/>
       <c r="N56" s="18"/>
       <c r="O56" s="16"/>
-      <c r="P56" s="20"/>
+      <c r="P56" s="19"/>
     </row>
     <row r="57" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A57" s="12">
-        <v>42480</v>
+        <v>45036</v>
       </c>
       <c r="B57" s="12"/>
       <c r="C57" s="18" t="s">
@@ -2259,8 +2254,8 @@
       </c>
       <c r="G57" s="16"/>
       <c r="H57" s="16"/>
-      <c r="I57" s="19">
-        <v>42480</v>
+      <c r="I57" s="17">
+        <v>45036</v>
       </c>
       <c r="J57" s="16"/>
       <c r="K57" s="18" t="s">
@@ -2270,11 +2265,11 @@
       <c r="M57" s="16"/>
       <c r="N57" s="18"/>
       <c r="O57" s="16"/>
-      <c r="P57" s="20"/>
+      <c r="P57" s="19"/>
     </row>
     <row r="58" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A58" s="12">
-        <v>42481</v>
+        <v>45037</v>
       </c>
       <c r="B58" s="12"/>
       <c r="C58" s="18" t="s">
@@ -2285,8 +2280,8 @@
       <c r="F58" s="18"/>
       <c r="G58" s="16"/>
       <c r="H58" s="16"/>
-      <c r="I58" s="19">
-        <v>42481</v>
+      <c r="I58" s="17">
+        <v>45037</v>
       </c>
       <c r="J58" s="16"/>
       <c r="K58" s="18" t="s">
@@ -2296,11 +2291,11 @@
       <c r="M58" s="16"/>
       <c r="N58" s="18"/>
       <c r="O58" s="16"/>
-      <c r="P58" s="20"/>
+      <c r="P58" s="19"/>
     </row>
     <row r="59" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A59" s="12">
-        <v>42482</v>
+        <v>45038</v>
       </c>
       <c r="B59" s="12"/>
       <c r="C59" s="18" t="s">
@@ -2313,8 +2308,8 @@
       </c>
       <c r="G59" s="16"/>
       <c r="H59" s="16"/>
-      <c r="I59" s="19">
-        <v>42482</v>
+      <c r="I59" s="17">
+        <v>45038</v>
       </c>
       <c r="J59" s="16"/>
       <c r="K59" s="18" t="s">
@@ -2326,14 +2321,14 @@
         <v>30</v>
       </c>
       <c r="O59" s="16"/>
-      <c r="P59" s="20"/>
+      <c r="P59" s="19"/>
     </row>
     <row r="60" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A60" s="12">
-        <v>42483</v>
+        <v>45039</v>
       </c>
       <c r="B60" s="12"/>
-      <c r="C60" s="32" t="s">
+      <c r="C60" s="30" t="s">
         <v>14</v>
       </c>
       <c r="D60" s="16"/>
@@ -2341,38 +2336,38 @@
       <c r="F60" s="18"/>
       <c r="G60" s="16"/>
       <c r="H60" s="16"/>
-      <c r="I60" s="19">
-        <v>42483</v>
+      <c r="I60" s="17">
+        <v>45039</v>
       </c>
       <c r="J60" s="16"/>
-      <c r="K60" s="32" t="s">
+      <c r="K60" s="30" t="s">
         <v>14</v>
       </c>
       <c r="L60" s="16"/>
       <c r="M60" s="16"/>
       <c r="N60" s="18"/>
       <c r="O60" s="16"/>
-      <c r="P60" s="20"/>
+      <c r="P60" s="19"/>
     </row>
     <row r="61" spans="1:16" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A61" s="12">
-        <v>42484</v>
-      </c>
-      <c r="B61" s="22"/>
+        <v>45040</v>
+      </c>
+      <c r="B61" s="21"/>
       <c r="C61" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="D61" s="28"/>
+      <c r="D61" s="26"/>
       <c r="E61" s="16"/>
       <c r="F61" s="18" t="s">
         <v>18</v>
       </c>
       <c r="G61" s="16"/>
       <c r="H61" s="16"/>
-      <c r="I61" s="19">
-        <v>42484</v>
-      </c>
-      <c r="J61" s="20"/>
+      <c r="I61" s="17">
+        <v>45040</v>
+      </c>
+      <c r="J61" s="19"/>
       <c r="K61" s="16" t="s">
         <v>32</v>
       </c>
@@ -2382,11 +2377,11 @@
         <v>33</v>
       </c>
       <c r="O61" s="16"/>
-      <c r="P61" s="20"/>
+      <c r="P61" s="19"/>
     </row>
     <row r="62" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A62" s="12">
-        <v>42485</v>
+        <v>45041</v>
       </c>
       <c r="B62" s="12"/>
       <c r="C62" s="18" t="s">
@@ -2399,8 +2394,8 @@
       </c>
       <c r="G62" s="16"/>
       <c r="H62" s="16"/>
-      <c r="I62" s="19">
-        <v>42485</v>
+      <c r="I62" s="17">
+        <v>45041</v>
       </c>
       <c r="J62" s="16"/>
       <c r="K62" s="18" t="s">
@@ -2412,11 +2407,11 @@
         <v>49</v>
       </c>
       <c r="O62" s="16"/>
-      <c r="P62" s="20"/>
+      <c r="P62" s="19"/>
     </row>
     <row r="63" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A63" s="12">
-        <v>42486</v>
+        <v>45042</v>
       </c>
       <c r="B63" s="12"/>
       <c r="C63" s="18" t="s">
@@ -2429,8 +2424,8 @@
       </c>
       <c r="G63" s="16"/>
       <c r="H63" s="16"/>
-      <c r="I63" s="19">
-        <v>42486</v>
+      <c r="I63" s="17">
+        <v>45042</v>
       </c>
       <c r="K63" s="18" t="s">
         <v>13</v>
@@ -2445,7 +2440,7 @@
     </row>
     <row r="64" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A64" s="12">
-        <v>42487</v>
+        <v>45043</v>
       </c>
       <c r="B64" s="12"/>
       <c r="C64" s="18" t="s">
@@ -2458,60 +2453,60 @@
       </c>
       <c r="G64" s="16"/>
       <c r="H64" s="16"/>
-      <c r="I64" s="19">
-        <v>42487</v>
-      </c>
-      <c r="K64" s="21" t="s">
+      <c r="I64" s="17">
+        <v>45043</v>
+      </c>
+      <c r="K64" s="20" t="s">
         <v>36</v>
       </c>
       <c r="L64" s="16"/>
       <c r="M64" s="16"/>
-      <c r="N64" s="21" t="s">
+      <c r="N64" s="20" t="s">
         <v>37</v>
       </c>
       <c r="O64" s="16"/>
-      <c r="P64" s="20"/>
+      <c r="P64" s="19"/>
     </row>
     <row r="65" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A65" s="12">
-        <v>42488</v>
+        <v>45044</v>
       </c>
       <c r="B65" s="12"/>
       <c r="C65" s="18" t="s">
         <v>38</v>
       </c>
       <c r="D65" s="16"/>
-      <c r="E65" s="20"/>
+      <c r="E65" s="19"/>
       <c r="F65" s="18"/>
       <c r="G65" s="16"/>
       <c r="H65" s="16"/>
-      <c r="I65" s="19">
-        <v>42488</v>
+      <c r="I65" s="17">
+        <v>45044</v>
       </c>
       <c r="K65" s="18" t="s">
         <v>38</v>
       </c>
       <c r="L65" s="16"/>
       <c r="M65" s="16"/>
-      <c r="N65" s="21"/>
+      <c r="N65" s="20"/>
       <c r="O65" s="16"/>
-      <c r="P65" s="20"/>
+      <c r="P65" s="19"/>
     </row>
     <row r="66" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A66" s="12">
-        <v>42489</v>
-      </c>
-      <c r="B66" s="22"/>
+        <v>45045</v>
+      </c>
+      <c r="B66" s="21"/>
       <c r="C66" s="18" t="s">
         <v>39</v>
       </c>
       <c r="D66" s="16"/>
-      <c r="E66" s="20"/>
+      <c r="E66" s="19"/>
       <c r="F66" s="16"/>
       <c r="G66" s="16"/>
       <c r="H66" s="16"/>
-      <c r="I66" s="19">
-        <v>42489</v>
+      <c r="I66" s="17">
+        <v>45045</v>
       </c>
       <c r="K66" s="18" t="s">
         <v>39</v>
@@ -2520,429 +2515,429 @@
       <c r="M66" s="16"/>
       <c r="N66" s="18"/>
       <c r="O66" s="16"/>
-      <c r="P66" s="20"/>
+      <c r="P66" s="19"/>
     </row>
     <row r="67" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A67" s="12">
-        <v>42490</v>
-      </c>
-      <c r="B67" s="22"/>
-      <c r="C67" s="36" t="s">
+        <v>45046</v>
+      </c>
+      <c r="B67" s="21"/>
+      <c r="C67" s="34" t="s">
         <v>14</v>
       </c>
       <c r="D67" s="16"/>
-      <c r="E67" s="20"/>
+      <c r="E67" s="19"/>
       <c r="F67" s="16"/>
       <c r="G67" s="16"/>
-      <c r="H67" s="20"/>
-      <c r="I67" s="12">
-        <v>42490</v>
+      <c r="H67" s="19"/>
+      <c r="I67" s="17">
+        <v>45046</v>
       </c>
       <c r="J67" s="3"/>
-      <c r="K67" s="36" t="s">
+      <c r="K67" s="34" t="s">
         <v>14</v>
       </c>
       <c r="L67" s="16"/>
-      <c r="M67" s="20"/>
+      <c r="M67" s="19"/>
       <c r="N67" s="16"/>
       <c r="O67" s="16"/>
-      <c r="P67" s="20"/>
+      <c r="P67" s="19"/>
     </row>
     <row r="68" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A68" s="12">
-        <v>43586</v>
-      </c>
-      <c r="B68" s="22"/>
-      <c r="C68" s="36" t="s">
+        <v>45047</v>
+      </c>
+      <c r="B68" s="21"/>
+      <c r="C68" s="34" t="s">
         <v>40</v>
       </c>
       <c r="D68" s="16"/>
-      <c r="E68" s="20"/>
+      <c r="E68" s="19"/>
       <c r="F68" s="16"/>
       <c r="G68" s="16"/>
-      <c r="H68" s="20"/>
-      <c r="I68" s="12">
-        <v>43586</v>
+      <c r="H68" s="19"/>
+      <c r="I68" s="17">
+        <v>45047</v>
       </c>
       <c r="J68" s="3"/>
-      <c r="K68" s="36" t="s">
+      <c r="K68" s="34" t="s">
         <v>40</v>
       </c>
       <c r="L68" s="16"/>
-      <c r="M68" s="20"/>
+      <c r="M68" s="19"/>
       <c r="N68" s="16"/>
       <c r="O68" s="16"/>
-      <c r="P68" s="20"/>
+      <c r="P68" s="19"/>
     </row>
     <row r="69" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A69" s="12">
-        <v>43587</v>
+        <v>45048</v>
       </c>
       <c r="B69" s="3"/>
       <c r="C69" s="16" t="s">
         <v>41</v>
       </c>
       <c r="D69" s="16"/>
-      <c r="E69" s="20"/>
+      <c r="E69" s="19"/>
       <c r="F69" s="18" t="s">
         <v>42</v>
       </c>
       <c r="G69" s="16"/>
-      <c r="H69" s="20"/>
-      <c r="I69" s="19">
-        <v>43587</v>
+      <c r="H69" s="19"/>
+      <c r="I69" s="17">
+        <v>45048</v>
       </c>
       <c r="J69" s="3"/>
       <c r="K69" s="16" t="s">
         <v>41</v>
       </c>
       <c r="L69" s="16"/>
-      <c r="M69" s="35"/>
+      <c r="M69" s="33"/>
       <c r="N69" s="18" t="s">
         <v>42</v>
       </c>
       <c r="O69" s="16"/>
-      <c r="P69" s="20"/>
+      <c r="P69" s="19"/>
     </row>
     <row r="70" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A70" s="19">
-        <v>43588</v>
+      <c r="A70" s="12">
+        <v>45049</v>
       </c>
       <c r="B70" s="3"/>
       <c r="C70" s="16" t="s">
         <v>36</v>
       </c>
       <c r="D70" s="16"/>
-      <c r="E70" s="20"/>
-      <c r="F70" s="21" t="s">
+      <c r="E70" s="19"/>
+      <c r="F70" s="20" t="s">
         <v>43</v>
       </c>
       <c r="G70" s="16"/>
-      <c r="H70" s="20"/>
-      <c r="I70" s="19">
-        <v>43588</v>
+      <c r="H70" s="19"/>
+      <c r="I70" s="17">
+        <v>45049</v>
       </c>
       <c r="J70" s="3"/>
       <c r="K70" s="16" t="s">
         <v>36</v>
       </c>
       <c r="L70" s="16"/>
-      <c r="M70" s="20"/>
+      <c r="M70" s="19"/>
       <c r="N70" s="18" t="s">
         <v>43</v>
       </c>
       <c r="O70" s="16"/>
-      <c r="P70" s="20"/>
+      <c r="P70" s="19"/>
     </row>
     <row r="71" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A71" s="19">
-        <v>43589</v>
+      <c r="A71" s="12">
+        <v>45050</v>
       </c>
       <c r="B71" s="3"/>
       <c r="C71" s="16" t="s">
         <v>13</v>
       </c>
       <c r="D71" s="16"/>
-      <c r="E71" s="20"/>
+      <c r="E71" s="19"/>
       <c r="F71" s="18" t="s">
         <v>13</v>
       </c>
       <c r="G71" s="16"/>
-      <c r="H71" s="20"/>
-      <c r="I71" s="19">
-        <v>43589</v>
+      <c r="H71" s="19"/>
+      <c r="I71" s="17">
+        <v>45050</v>
       </c>
       <c r="J71" s="3"/>
       <c r="K71" s="16" t="s">
         <v>13</v>
       </c>
       <c r="L71" s="16"/>
-      <c r="M71" s="20"/>
+      <c r="M71" s="19"/>
       <c r="N71" s="18"/>
       <c r="O71" s="16"/>
-      <c r="P71" s="20"/>
+      <c r="P71" s="19"/>
     </row>
     <row r="72" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A72" s="19">
-        <v>43590</v>
+      <c r="A72" s="12">
+        <v>45051</v>
       </c>
       <c r="B72" s="3"/>
       <c r="C72" s="18" t="s">
         <v>13</v>
       </c>
       <c r="D72" s="16"/>
-      <c r="E72" s="20"/>
+      <c r="E72" s="19"/>
       <c r="F72" s="18" t="s">
         <v>13</v>
       </c>
       <c r="G72" s="16"/>
-      <c r="H72" s="20"/>
-      <c r="I72" s="19">
-        <v>43590</v>
+      <c r="H72" s="19"/>
+      <c r="I72" s="17">
+        <v>45051</v>
       </c>
       <c r="J72" s="3"/>
       <c r="K72" s="18" t="s">
         <v>13</v>
       </c>
       <c r="L72" s="16"/>
-      <c r="M72" s="20"/>
+      <c r="M72" s="19"/>
       <c r="N72" s="18"/>
       <c r="O72" s="16"/>
-      <c r="P72" s="20"/>
+      <c r="P72" s="19"/>
     </row>
     <row r="73" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A73" s="19">
-        <v>43591</v>
+      <c r="A73" s="12">
+        <v>45052</v>
       </c>
       <c r="B73" s="3"/>
       <c r="C73" s="18" t="s">
         <v>13</v>
       </c>
       <c r="D73" s="16"/>
-      <c r="E73" s="20"/>
+      <c r="E73" s="19"/>
       <c r="F73" s="18" t="s">
         <v>13</v>
       </c>
       <c r="G73" s="16"/>
-      <c r="H73" s="20"/>
-      <c r="I73" s="19">
-        <v>43591</v>
+      <c r="H73" s="19"/>
+      <c r="I73" s="17">
+        <v>45052</v>
       </c>
       <c r="J73" s="3"/>
       <c r="K73" s="18" t="s">
         <v>13</v>
       </c>
       <c r="L73" s="16"/>
-      <c r="M73" s="20"/>
+      <c r="M73" s="19"/>
       <c r="N73" s="18"/>
       <c r="O73" s="16"/>
-      <c r="P73" s="20"/>
+      <c r="P73" s="19"/>
     </row>
     <row r="74" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A74" s="19">
-        <v>43592</v>
+      <c r="A74" s="12">
+        <v>45053</v>
       </c>
       <c r="B74" s="3"/>
-      <c r="C74" s="32" t="s">
+      <c r="C74" s="30" t="s">
         <v>14</v>
       </c>
       <c r="D74" s="16"/>
-      <c r="E74" s="20"/>
+      <c r="E74" s="19"/>
       <c r="F74" s="18"/>
       <c r="G74" s="16"/>
-      <c r="H74" s="20"/>
-      <c r="I74" s="19">
-        <v>43592</v>
+      <c r="H74" s="19"/>
+      <c r="I74" s="17">
+        <v>45053</v>
       </c>
       <c r="J74" s="3"/>
-      <c r="K74" s="32" t="s">
+      <c r="K74" s="30" t="s">
         <v>24</v>
       </c>
       <c r="L74" s="16"/>
-      <c r="M74" s="20"/>
+      <c r="M74" s="19"/>
       <c r="N74" s="18"/>
       <c r="O74" s="16"/>
-      <c r="P74" s="20"/>
+      <c r="P74" s="19"/>
     </row>
     <row r="75" spans="1:16" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A75" s="19">
-        <v>43593</v>
+      <c r="A75" s="12">
+        <v>45054</v>
       </c>
       <c r="B75" s="3"/>
       <c r="C75" s="18" t="s">
         <v>13</v>
       </c>
       <c r="D75" s="16"/>
-      <c r="E75" s="20"/>
+      <c r="E75" s="19"/>
       <c r="F75" s="18" t="s">
         <v>13</v>
       </c>
       <c r="G75" s="16"/>
-      <c r="H75" s="20"/>
-      <c r="I75" s="19">
-        <v>43593</v>
+      <c r="H75" s="19"/>
+      <c r="I75" s="17">
+        <v>45054</v>
       </c>
       <c r="J75" s="3"/>
-      <c r="K75" s="29" t="s">
+      <c r="K75" s="27" t="s">
         <v>9</v>
       </c>
       <c r="L75" s="16"/>
-      <c r="M75" s="20"/>
+      <c r="M75" s="19"/>
       <c r="N75" s="18" t="s">
         <v>44</v>
       </c>
       <c r="O75" s="16"/>
-      <c r="P75" s="20"/>
+      <c r="P75" s="19"/>
     </row>
     <row r="76" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A76" s="19">
-        <v>43594</v>
+      <c r="A76" s="12">
+        <v>45055</v>
       </c>
       <c r="B76" s="3"/>
       <c r="C76" s="18" t="s">
         <v>45</v>
       </c>
       <c r="D76" s="16"/>
-      <c r="E76" s="20"/>
+      <c r="E76" s="19"/>
       <c r="F76" s="18" t="s">
         <v>45</v>
       </c>
       <c r="G76" s="16"/>
-      <c r="H76" s="20"/>
-      <c r="I76" s="19">
-        <v>43594</v>
+      <c r="H76" s="19"/>
+      <c r="I76" s="17">
+        <v>45055</v>
       </c>
       <c r="J76" s="3"/>
       <c r="K76" s="18" t="s">
         <v>28</v>
       </c>
       <c r="L76" s="16"/>
-      <c r="M76" s="20"/>
+      <c r="M76" s="19"/>
       <c r="N76" s="18"/>
       <c r="O76" s="16"/>
-      <c r="P76" s="20"/>
+      <c r="P76" s="19"/>
     </row>
     <row r="77" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A77" s="19">
-        <v>43595</v>
+      <c r="A77" s="12">
+        <v>45056</v>
       </c>
       <c r="B77" s="3"/>
       <c r="C77" s="18" t="s">
         <v>45</v>
       </c>
       <c r="D77" s="16"/>
-      <c r="E77" s="20"/>
+      <c r="E77" s="19"/>
       <c r="F77" s="18" t="s">
         <v>45</v>
       </c>
       <c r="G77" s="16"/>
-      <c r="H77" s="20"/>
-      <c r="I77" s="19">
-        <v>43595</v>
+      <c r="H77" s="19"/>
+      <c r="I77" s="17">
+        <v>45056</v>
       </c>
       <c r="J77" s="3"/>
       <c r="K77" s="18" t="s">
         <v>46</v>
       </c>
       <c r="L77" s="16"/>
-      <c r="M77" s="20"/>
+      <c r="M77" s="19"/>
       <c r="N77" s="18"/>
       <c r="O77" s="16"/>
-      <c r="P77" s="20"/>
+      <c r="P77" s="19"/>
     </row>
     <row r="78" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A78" s="19">
-        <v>43596</v>
+      <c r="A78" s="12">
+        <v>45057</v>
       </c>
       <c r="B78" s="3"/>
       <c r="C78" s="18" t="s">
         <v>45</v>
       </c>
       <c r="D78" s="16"/>
-      <c r="E78" s="20"/>
+      <c r="E78" s="19"/>
       <c r="F78" s="18" t="s">
         <v>45</v>
       </c>
       <c r="G78" s="16"/>
-      <c r="H78" s="20"/>
-      <c r="I78" s="19">
-        <v>43596</v>
+      <c r="H78" s="19"/>
+      <c r="I78" s="17">
+        <v>45057</v>
       </c>
       <c r="J78" s="3"/>
       <c r="K78" s="18" t="s">
         <v>46</v>
       </c>
       <c r="L78" s="16"/>
-      <c r="M78" s="20"/>
+      <c r="M78" s="19"/>
       <c r="N78" s="18"/>
       <c r="O78" s="16"/>
-      <c r="P78" s="20"/>
+      <c r="P78" s="19"/>
     </row>
     <row r="79" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A79" s="19">
-        <v>43597</v>
+      <c r="A79" s="12">
+        <v>45058</v>
       </c>
       <c r="B79" s="3"/>
       <c r="C79" s="18" t="s">
         <v>45</v>
       </c>
       <c r="D79" s="16"/>
-      <c r="E79" s="20"/>
+      <c r="E79" s="19"/>
       <c r="F79" s="18" t="s">
         <v>45</v>
       </c>
       <c r="G79" s="16"/>
-      <c r="H79" s="20"/>
-      <c r="I79" s="19">
-        <v>43597</v>
+      <c r="H79" s="19"/>
+      <c r="I79" s="17">
+        <v>45058</v>
       </c>
       <c r="J79" s="3"/>
       <c r="K79" s="18" t="s">
         <v>28</v>
       </c>
       <c r="L79" s="16"/>
-      <c r="M79" s="20"/>
+      <c r="M79" s="19"/>
       <c r="N79" s="18"/>
       <c r="O79" s="16"/>
-      <c r="P79" s="20"/>
+      <c r="P79" s="19"/>
     </row>
     <row r="80" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A80" s="19">
-        <v>43598</v>
+      <c r="A80" s="12">
+        <v>45059</v>
       </c>
       <c r="B80" s="3"/>
       <c r="C80" s="18" t="s">
         <v>13</v>
       </c>
       <c r="D80" s="16"/>
-      <c r="E80" s="20"/>
+      <c r="E80" s="19"/>
       <c r="F80" s="18" t="s">
         <v>13</v>
       </c>
       <c r="G80" s="16"/>
-      <c r="H80" s="20"/>
-      <c r="I80" s="19">
-        <v>43598</v>
+      <c r="H80" s="19"/>
+      <c r="I80" s="17">
+        <v>45059</v>
       </c>
       <c r="J80" s="3"/>
       <c r="K80" s="18" t="s">
         <v>28</v>
       </c>
       <c r="L80" s="16"/>
-      <c r="M80" s="20"/>
+      <c r="M80" s="19"/>
       <c r="N80" s="18"/>
       <c r="O80" s="16"/>
-      <c r="P80" s="20"/>
+      <c r="P80" s="19"/>
     </row>
     <row r="81" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A81" s="19">
-        <v>43599</v>
+      <c r="A81" s="12">
+        <v>45060</v>
       </c>
       <c r="B81" s="3"/>
-      <c r="C81" s="32" t="s">
+      <c r="C81" s="30" t="s">
         <v>14</v>
       </c>
       <c r="D81" s="16"/>
-      <c r="E81" s="20"/>
+      <c r="E81" s="19"/>
       <c r="F81" s="18"/>
       <c r="G81" s="16"/>
-      <c r="H81" s="20"/>
-      <c r="I81" s="19">
-        <v>43599</v>
+      <c r="H81" s="19"/>
+      <c r="I81" s="17">
+        <v>45060</v>
       </c>
       <c r="J81" s="3"/>
-      <c r="K81" s="32" t="s">
+      <c r="K81" s="30" t="s">
         <v>14</v>
       </c>
       <c r="L81" s="16"/>
-      <c r="M81" s="20"/>
+      <c r="M81" s="19"/>
       <c r="N81" s="18"/>
       <c r="O81" s="16"/>
-      <c r="P81" s="20"/>
+      <c r="P81" s="19"/>
     </row>
     <row r="82" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A82" s="19">
-        <v>43600</v>
+      <c r="A82" s="12">
+        <v>45061</v>
       </c>
       <c r="B82" s="3"/>
       <c r="C82" s="18" t="s">
@@ -2955,40 +2950,40 @@
       </c>
       <c r="G82" s="16"/>
       <c r="H82" s="16"/>
-      <c r="I82" s="19">
-        <v>43600</v>
+      <c r="I82" s="17">
+        <v>45061</v>
       </c>
       <c r="J82" s="3"/>
       <c r="K82" s="18" t="s">
         <v>38</v>
       </c>
       <c r="L82" s="16"/>
-      <c r="M82" s="20"/>
+      <c r="M82" s="19"/>
     </row>
     <row r="83" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A83" s="37">
+      <c r="A83" s="12">
         <v>45062</v>
       </c>
-      <c r="B83" s="30"/>
+      <c r="B83" s="28"/>
       <c r="C83" s="18" t="s">
         <v>47</v>
       </c>
       <c r="D83" s="16"/>
-      <c r="E83" s="20"/>
+      <c r="E83" s="19"/>
       <c r="F83" s="18" t="s">
         <v>47</v>
       </c>
       <c r="G83" s="16"/>
-      <c r="H83" s="20"/>
-      <c r="I83" s="37">
+      <c r="H83" s="19"/>
+      <c r="I83" s="17">
         <v>45062</v>
       </c>
-      <c r="J83" s="30"/>
-      <c r="K83" s="33" t="s">
+      <c r="J83" s="28"/>
+      <c r="K83" s="31" t="s">
         <v>47</v>
       </c>
-      <c r="L83" s="39"/>
-      <c r="M83" s="38"/>
+      <c r="L83" s="36"/>
+      <c r="M83" s="35"/>
       <c r="N83" s="14"/>
     </row>
   </sheetData>

</xml_diff>